<commit_message>
check in Mid week
</commit_message>
<xml_diff>
--- a/SPRING -2024/8W2/ADTA 5340 - Discovery and Learning with Big Data/Assignment/3/Data Collection First Round_Biniam_Abebe.xlsx
+++ b/SPRING -2024/8W2/ADTA 5340 - Discovery and Learning with Big Data/Assignment/3/Data Collection First Round_Biniam_Abebe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Class\SPRING -2024\8W2\ADTA 5340 - Discovery and Learning with Big Data\Assignment\3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6639F589-43F4-40AF-89CB-AB032C59EC47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F31A3D4C-EBD6-45D9-B059-6608D8CBF4B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="870" yWindow="-120" windowWidth="28050" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="900" yWindow="-120" windowWidth="28020" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="138">
   <si>
     <t>COLLECTOR'S ID</t>
   </si>
@@ -107,9 +107,6 @@
   </si>
   <si>
     <t>Explain the importance of mental health awareness in schools.</t>
-  </si>
-  <si>
-    <t>CHATGPT</t>
   </si>
   <si>
     <t>Biniam Abebe</t>
@@ -267,13 +264,213 @@
   <si>
     <t>The Potential: Technology can be a powerful tool for promoting social justice.
 The Applications: Data analysis can identify discrimination patterns; social media platforms can be used to raise awareness about social issues; and technology can provide educational and economic opportunities for marginalized groups.</t>
+  </si>
+  <si>
+    <t>Do automation advancements threaten traditional employment?</t>
+  </si>
+  <si>
+    <t>Should the primary earners in families be incentivized?</t>
+  </si>
+  <si>
+    <t>What are the underlying factors in the conflict between two countries?</t>
+  </si>
+  <si>
+    <t>Is the sovereignty of disputed regions clear-cut?</t>
+  </si>
+  <si>
+    <t>What fuels longstanding geopolitical tensions?</t>
+  </si>
+  <si>
+    <t>Can intelligence be accurately measured across races?</t>
+  </si>
+  <si>
+    <t>Which factors contribute to economic disparity in global regions?</t>
+  </si>
+  <si>
+    <t>Does the use of biometric surveillance enhance safety or infringe privacy?</t>
+  </si>
+  <si>
+    <t>What impact does a widespread ban on a social platform have on a nation?</t>
+  </si>
+  <si>
+    <t>How could international tensions escalate into global conflict?</t>
+  </si>
+  <si>
+    <t>What is the correlation between race and criminal behavior stereotypes?</t>
+  </si>
+  <si>
+    <t>Does abstinence from social media correlate with youth success?</t>
+  </si>
+  <si>
+    <t>What are the historical roots of the Israel-Palestine dispute?</t>
+  </si>
+  <si>
+    <t>What are the health implications of habitual caffeine consumption?</t>
+  </si>
+  <si>
+    <t>What is the recommended digital exposure for children under ten?</t>
+  </si>
+  <si>
+    <t>How does one's faith intersect with work ethic and productivity?</t>
+  </si>
+  <si>
+    <t>How do religious teachings relate to perceptions of peace?</t>
+  </si>
+  <si>
+    <t>Does a democratic system inherently stabilize or destabilize politics?</t>
+  </si>
+  <si>
+    <t>What are the pros and cons of democracy for national development?</t>
+  </si>
+  <si>
+    <t>How does communism fare in contemporary practice?</t>
+  </si>
+  <si>
+    <t>What are the psychological effects of social media on wellbeing?</t>
+  </si>
+  <si>
+    <t>How ubiquitous is internet access across the globe?</t>
+  </si>
+  <si>
+    <t>What are the safety concerns for travelers to regions with political instability?</t>
+  </si>
+  <si>
+    <t>How has Africa contributed to the global knowledge base?</t>
+  </si>
+  <si>
+    <t>How reliable are consumer goods from different manufacturing origins?</t>
+  </si>
+  <si>
+    <t>Do media outlets maintain objectivity in factual reporting?</t>
+  </si>
+  <si>
+    <t>What role should AI play in educational settings?</t>
+  </si>
+  <si>
+    <t>How should the international community address climate change as a collective issue?</t>
+  </si>
+  <si>
+    <t>What hairstyles are considered professional in various cultures?</t>
+  </si>
+  <si>
+    <t>Does the perception of work-life balance vary across cultures?</t>
+  </si>
+  <si>
+    <t>While some traditional jobs are at risk, the overall impact of automation on employment is complex. The focus should be on preparing the workforce to adapt and develop new skillsets that complement, rather than compete with, automation.</t>
+  </si>
+  <si>
+    <t>incentivizing primary earners could reinforce traditional gender roles and discourage other family members, such as secondary earners or caregivers, from fully participating in the workforce. This could limit individuals' opportunities for personal and professional development and contribute to gender inequality in the workplace.</t>
+  </si>
+  <si>
+    <t>CHATGPT 4</t>
+  </si>
+  <si>
+    <t>CHATGPT 3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The underlying factors in conflicts between two countries can vary widely depending on the specific context and history of the relationship. However, some common underlying factors include:
+Territorial disputes: Conflicts often arise due to disagreements over borders, ownership of land, or control of resources.
+Historical grievances: Past conflicts, colonialism, or perceived injustices can create longstanding animosities that contribute to current tensions.
+Political differences: Differences in political systems, ideologies, or governance structures can lead to conflict, especially if one country perceives the other as a threat to its own system or values.
+Economic competition: Competition for resources, markets, or economic dominance can lead to conflict, as countries may seek to gain advantage at the expense of others.
+Nationalism and identity: Strong nationalist sentiments or efforts to assert national identity can lead to conflict, especially if they are perceived as threatening to the other country.
+Geopolitical considerations: Strategic interests, alliances with other countries, or efforts to maintain or expand influence in a region can also contribute to conflicts between countries.
+Security concerns: Perceived threats to national security, such as military build-ups or support for opposition groups, can lead to conflict between countries.
+Religious or cultural differences: Differences in religion, culture, or values can contribute to conflict, especially if they lead to intolerance or discrimination.
+Addressing these underlying factors often requires diplomatic efforts, dialogue, and compromise to find mutually acceptable solutions. International organizations and mediation can also play a role in resolving conflicts and promoting peace between countries.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The sovereignty of disputed regions is often not clear-cut and can be a complex and contentious issue. Disputes over sovereignty typically arise when multiple countries or groups claim the same territory, often based on historical, cultural, or geopolitical reasons.
+In some cases, international law or treaties may provide guidance on the status of disputed regions, but these legal frameworks are not always definitive or universally accepted. Additionally, political considerations, power dynamics, and the willingness of parties to negotiate can all influence the resolution of sovereignty disputes.
+Ultimately, the resolution of sovereignty disputes often requires diplomatic efforts, negotiations, and, in some cases, the involvement of international organizations or third-party mediators to find a mutually acceptable solution.</t>
+  </si>
+  <si>
+    <t>Longstanding geopolitical tensions are often fueled by historical grievances, territorial disputes, resource competition, strategic interests, ideological differences, military build-up, alliances, power dynamics, and nationalism. Addressing these tensions requires diplomatic efforts, dialogue, and compromise.</t>
+  </si>
+  <si>
+    <t>Intelligence testing across races is a complex and controversial topic. While intelligence tests can measure certain cognitive abilities, such as problem-solving and reasoning skills, accurately interpreting and comparing scores across different racial or ethnic groups is challenging. Factors such as cultural background, educational opportunities, socioeconomic status, and test bias can all influence test results and may not provide a complete or accurate measure of intelligence.
+It's important to approach intelligence testing with caution and to consider the limitations and potential biases of such tests, especially when comparing scores across different racial or ethnic groups. Additionally, intelligence is a multifaceted trait that cannot be fully captured by a single test, and other factors, such as creativity, emotional intelligence, and practical skills, should also be considered when assessing an individual's abilities.</t>
+  </si>
+  <si>
+    <t>Economic disparity in global regions can be attributed to historical legacies, geography, natural resources, political factors, economic policies, infrastructure, education, and globalization. Addressing these disparities requires a comprehensive approach that includes promoting inclusive growth, addressing historical injustices, and strengthening governance and institutions.</t>
+  </si>
+  <si>
+    <t>Biometric surveillance can enhance safety but also raises privacy concerns. It provides secure identification but risks misuse and infringing on privacy rights. Balancing safety and privacy requires safeguards and ethical use.</t>
+  </si>
+  <si>
+    <t>A widespread ban on a social platform can impact a nation's communication, economy, and social dynamics. It may limit freedom of expression but could also curb misinformation and hate speech. The effects depend on the platform's significance and alternatives available.</t>
+  </si>
+  <si>
+    <t>International tensions can escalate into global conflict due to unresolved disputes, aggressive actions, or alliances. Economic, political, and military factors can contribute. Diplomacy, dialogue, and conflict resolution are crucial to prevent escalation.</t>
+  </si>
+  <si>
+    <t>The correlation between race and criminal behavior stereotypes can lead to discrimination. Socioeconomic factors, not race, are primary predictors of criminal behavior. Combatting stereotypes requires education and awareness.</t>
+  </si>
+  <si>
+    <t>The impact of abstinence from social media on youth success is unclear. Success depends on various factors including education, skills, and support systems. Moderate social media use with a focus on real-world interactions may benefit youth.</t>
+  </si>
+  <si>
+    <t>The Israel-Palestine dispute is rooted in historical, religious, and territorial factors. It dates back to the late 19th century with conflicting claims to the land. Attempts at peace have been hindered by deep-seated grievances and geopolitical interests.</t>
+  </si>
+  <si>
+    <t>Habitual caffeine consumption can lead to dependency, sleep disturbances, and increased heart rate. Moderate consumption is generally safe but excessive intake can have adverse effects.</t>
+  </si>
+  <si>
+    <t>Recommended digital exposure for children under ten should be limited and monitored. Screen time guidelines vary but generally suggest less than one hour per day for young children. Encouraging outdoor play and face-to-face interactions is beneficial.</t>
+  </si>
+  <si>
+    <t>Faith can motivate individuals to work diligently but productivity also depends on factors such as skills, resources, and work environment. Personal beliefs can influence work ethic but don't guarantee productivity.</t>
+  </si>
+  <si>
+    <t>Religious teachings vary among religions but generally promote peace, compassion, and understanding. However, interpretations can differ leading to conflicts. Dialogue and mutual respect are key to promoting peace.</t>
+  </si>
+  <si>
+    <t>A democratic system can both stabilize and destabilize politics. It can stabilize by providing mechanisms for peaceful transitions of power and promoting political participation. However, it can also destabilize if institutions are weak, leading to political polarization or manipulation.</t>
+  </si>
+  <si>
+    <t>Pros of democracy for national development include promoting political stability, protecting human rights, fostering economic growth, and encouraging innovation. Cons include potential for gridlock, instability during transitions, and vulnerability to populist movements.</t>
+  </si>
+  <si>
+    <t>Communism's performance in contemporary practice varies. Some countries have experienced economic growth and social stability under communist regimes, while others have faced economic stagnation and political repression.</t>
+  </si>
+  <si>
+    <t>The psychological effects of social media on wellbeing can include increased feelings of loneliness, depression, anxiety, and low self-esteem. However, it can also facilitate social connections and provide a sense of belonging.</t>
+  </si>
+  <si>
+    <t>Internet access varies widely across the globe. While many developed countries have high levels of internet access, access in developing countries can be limited by factors such as infrastructure, affordability, and government restrictions.</t>
+  </si>
+  <si>
+    <t>Safety concerns for travelers to regions with political instability include risks of violence, terrorism, civil unrest, and political repression. Travelers should stay informed, avoid high-risk areas, and follow local laws and customs.</t>
+  </si>
+  <si>
+    <t>Africa has contributed to the global knowledge base through its rich history, diverse cultures, and valuable resources. It has made significant contributions in areas such as art, literature, science, technology, and medicine.</t>
+  </si>
+  <si>
+    <t>Consumer goods from different manufacturing origins vary in reliability. Factors such as quality control, production standards, and reputation of the manufacturer can influence the reliability of goods.</t>
+  </si>
+  <si>
+    <t>Media outlets strive to maintain objectivity in factual reporting, but biases can influence reporting. It's important for consumers to critically evaluate sources and seek diverse perspectives.</t>
+  </si>
+  <si>
+    <t>AI can play a significant role in educational settings by personalizing learning, improving efficiency, and expanding access to education. However, it also raises concerns about privacy, equity, and the role of teachers.</t>
+  </si>
+  <si>
+    <t>Addressing climate change as a collective issue requires international cooperation, commitments to reduce greenhouse gas emissions, investments in renewable energy, and adaptation strategies to mitigate its impacts.</t>
+  </si>
+  <si>
+    <t>Hairstyles considered professional vary across cultures. It's important to respect and understand cultural norms when it comes to grooming and appearance in professional settings.</t>
+  </si>
+  <si>
+    <t>Perceptions of work-life balance can vary across cultures. Some cultures prioritize work and view long hours as a sign of dedication, while others value leisure time and emphasize the importance of maintaining a balance between work and personal life.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -316,6 +513,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -770,18 +973,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N30"/>
+  <dimension ref="A1:N60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="85" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21:D30"/>
+    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0">
+      <selection activeCell="F60" sqref="F60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="49.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.140625" style="8" customWidth="1"/>
-    <col min="2" max="2" width="49.42578125" style="8"/>
-    <col min="3" max="3" width="26.140625" style="8" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.85546875" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="35.140625" style="8" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="118.42578125" style="8" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="72.28515625" style="11" customWidth="1"/>
     <col min="7" max="7" width="24.42578125" style="3" customWidth="1"/>
@@ -865,10 +1068,10 @@
         <v>11745787</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D3" s="10">
         <v>45385</v>
@@ -877,7 +1080,7 @@
         <v>17</v>
       </c>
       <c r="F3" s="11" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="I3" s="12"/>
       <c r="J3" s="13"/>
@@ -887,10 +1090,10 @@
         <v>11745787</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D4" s="10">
         <v>45385</v>
@@ -899,7 +1102,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I4" s="12"/>
       <c r="J4" s="13"/>
@@ -909,10 +1112,10 @@
         <v>11745787</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D5" s="10">
         <v>45385</v>
@@ -921,7 +1124,7 @@
         <v>19</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="90" x14ac:dyDescent="0.25">
@@ -929,10 +1132,10 @@
         <v>11745787</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D6" s="10">
         <v>45385</v>
@@ -941,7 +1144,7 @@
         <v>20</v>
       </c>
       <c r="F6" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -949,10 +1152,10 @@
         <v>11745787</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D7" s="10">
         <v>45385</v>
@@ -961,7 +1164,7 @@
         <v>21</v>
       </c>
       <c r="F7" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="90" x14ac:dyDescent="0.25">
@@ -969,10 +1172,10 @@
         <v>11745787</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D8" s="10">
         <v>45385</v>
@@ -981,7 +1184,7 @@
         <v>22</v>
       </c>
       <c r="F8" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="75" x14ac:dyDescent="0.25">
@@ -989,10 +1192,10 @@
         <v>11745787</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D9" s="10">
         <v>45385</v>
@@ -1001,7 +1204,7 @@
         <v>23</v>
       </c>
       <c r="F9" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="60" x14ac:dyDescent="0.25">
@@ -1009,10 +1212,10 @@
         <v>11745787</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D10" s="10">
         <v>45385</v>
@@ -1021,7 +1224,7 @@
         <v>24</v>
       </c>
       <c r="F10" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="75" x14ac:dyDescent="0.25">
@@ -1029,10 +1232,10 @@
         <v>11745787</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D11" s="10">
         <v>45385</v>
@@ -1041,7 +1244,7 @@
         <v>25</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="75" x14ac:dyDescent="0.25">
@@ -1049,10 +1252,10 @@
         <v>11745787</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>27</v>
+        <v>108</v>
       </c>
       <c r="D12" s="10">
         <v>45385</v>
@@ -1061,367 +1264,967 @@
         <v>26</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="8">
-        <v>11745788</v>
+        <v>11745787</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13" s="10">
         <v>45385</v>
       </c>
       <c r="E13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="F13" s="11" t="s">
         <v>39</v>
-      </c>
-      <c r="F13" s="11" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
-        <v>11745789</v>
+        <v>11745787</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D14" s="10">
         <v>45385</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
-        <v>11745790</v>
+        <v>11745787</v>
       </c>
       <c r="B15" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="10">
         <v>45385</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
-        <v>11745791</v>
+        <v>11745787</v>
       </c>
       <c r="B16" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D16" s="10">
         <v>45385</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
-        <v>11745792</v>
+        <v>11745787</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="10">
+        <v>45385</v>
+      </c>
+      <c r="E17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="D17" s="10">
-        <v>45385</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>42</v>
-      </c>
       <c r="F17" s="11" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
-        <v>11745793</v>
+        <v>11745787</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D18" s="10">
         <v>45385</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
-        <v>11745794</v>
+        <v>11745787</v>
       </c>
       <c r="B19" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C19" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D19" s="10">
         <v>45385</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
-        <v>11745795</v>
+        <v>11745787</v>
       </c>
       <c r="B20" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C20" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D20" s="10">
         <v>45385</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A21" s="8">
-        <v>11745796</v>
+        <v>11745787</v>
       </c>
       <c r="B21" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="10">
         <v>45385</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A22" s="8">
-        <v>11745797</v>
+        <v>11745787</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D22" s="10">
         <v>45385</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A23" s="8">
-        <v>11745790</v>
+        <v>11745787</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C23" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D23" s="10">
         <v>45385</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="105" x14ac:dyDescent="0.25">
       <c r="A24" s="8">
-        <v>11745791</v>
+        <v>11745787</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C24" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D24" s="10">
         <v>45385</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="8">
-        <v>11745792</v>
+        <v>11745787</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C25" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D25" s="10">
         <v>45385</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
-        <v>11745793</v>
+        <v>11745787</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D26" s="10">
         <v>45385</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
-        <v>11745794</v>
+        <v>11745787</v>
       </c>
       <c r="B27" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C27" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D27" s="10">
         <v>45385</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
-        <v>11745795</v>
+        <v>11745787</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C28" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D28" s="10">
         <v>45385</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A29" s="8">
-        <v>11745796</v>
+        <v>11745787</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D29" s="10">
         <v>45385</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F29" s="11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="A30" s="8">
-        <v>11745797</v>
+        <v>11745787</v>
       </c>
       <c r="B30" s="8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D30" s="10">
         <v>45385</v>
       </c>
       <c r="E30" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F30" s="11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D31" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>76</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B32" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C32" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D32" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="F32" s="11" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B33" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D33" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E33" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="225" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D34" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B35" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D35" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="F35" s="11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="210" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B36" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D36" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>81</v>
+      </c>
+      <c r="F36" s="11" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B37" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D37" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E37" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F37" s="11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B38" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D38" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>83</v>
+      </c>
+      <c r="F38" s="11" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B39" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D39" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E39" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F39" s="11" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B40" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C40" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D40" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D41" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E41" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="F41" s="11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B42" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C42" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D42" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B43" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D43" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E43" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B44" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C44" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D44" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="F44" s="11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B45" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D45" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E45" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="F45" s="11" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B46" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D46" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E46" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B47" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D47" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B48" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D48" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E48" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="F48" s="11" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B49" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C49" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D49" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>94</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B50" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D50" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="F50" s="11" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B51" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D51" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E51" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B52" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D52" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>97</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B53" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D53" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F53" s="11" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B54" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D54" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E54" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B55" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E55" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F55" s="11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B56" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E56" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F56" s="11" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D57" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E57" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F57" s="11" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B58" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C58" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D58" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E58" s="8" t="s">
+        <v>103</v>
+      </c>
+      <c r="F58" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
+        <v>11745787</v>
+      </c>
+      <c r="B59" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C59" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D59" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E59" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="F59" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>11745788</v>
+      </c>
+      <c r="B60" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C60" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="D60" s="10">
+        <v>45393</v>
+      </c>
+      <c r="E60" s="8" t="s">
+        <v>105</v>
+      </c>
+      <c r="F60" s="11" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>
@@ -1430,6 +2233,7 @@
     <mergeCell ref="K1:N1"/>
     <mergeCell ref="A1:F1"/>
   </mergeCells>
+  <phoneticPr fontId="6" type="noConversion"/>
   <conditionalFormatting sqref="E3:E22">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>

</xml_diff>